<commit_message>
add cust main data input
</commit_message>
<xml_diff>
--- a/Data Files/LOS_CompanyCustomer_TestData.xlsx
+++ b/Data Files/LOS_CompanyCustomer_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="201">
   <si>
     <t xml:space="preserve">ScenarioId</t>
   </si>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">3703283107950004</t>
   </si>
   <si>
-    <t xml:space="preserve">DataNo</t>
-  </si>
-  <si>
     <t xml:space="preserve">NextToNewApplication</t>
   </si>
   <si>
@@ -171,6 +168,12 @@
     <t xml:space="preserve">BANK</t>
   </si>
   <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABCDEXYZ</t>
   </si>
   <si>
@@ -178,6 +181,18 @@
   </si>
   <si>
     <t xml:space="preserve">QATest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000</t>
   </si>
   <si>
     <t xml:space="preserve">AddressTypeName</t>
@@ -733,7 +748,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,8 +1066,8 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1183,8 +1198,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1202,179 +1217,179 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>45292</v>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>45292</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>45292</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>45292</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0</v>
+      <c r="H5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1396,7 +1411,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1406,80 +1421,80 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="4" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
@@ -1491,31 +1506,31 @@
         <v>15820</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="1" t="n">
         <v>0</v>
@@ -1524,24 +1539,24 @@
         <v>60</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>5</v>
@@ -1553,31 +1568,31 @@
         <v>15820</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>0</v>
@@ -1586,24 +1601,24 @@
         <v>60</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -1615,31 +1630,31 @@
         <v>15820</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>0</v>
@@ -1648,24 +1663,24 @@
         <v>60</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>5</v>
@@ -1677,31 +1692,31 @@
         <v>15820</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>0</v>
@@ -1710,24 +1725,24 @@
         <v>60</v>
       </c>
       <c r="S5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>3</v>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -1739,31 +1754,31 @@
         <v>15820</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="1" t="n">
         <v>0</v>
@@ -1772,24 +1787,24 @@
         <v>60</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>5</v>
@@ -1801,31 +1816,31 @@
         <v>15820</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="1" t="n">
         <v>0</v>
@@ -1834,24 +1849,24 @@
         <v>60</v>
       </c>
       <c r="S7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -1863,31 +1878,31 @@
         <v>15820</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q8" s="1" t="n">
         <v>0</v>
@@ -1896,24 +1911,24 @@
         <v>60</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>5</v>
@@ -1925,31 +1940,31 @@
         <v>15820</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Q9" s="1" t="n">
         <v>0</v>
@@ -1958,13 +1973,13 @@
         <v>60</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +2001,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1998,24 +2013,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,10 +2038,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>60</v>
@@ -2045,10 +2060,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>40</v>
@@ -2067,10 +2082,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>100</v>
@@ -2089,10 +2104,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>60</v>
@@ -2111,10 +2126,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>40</v>
@@ -2133,10 +2148,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>100</v>
@@ -2169,7 +2184,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2180,42 +2195,42 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="7" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,19 +2238,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,19 +2258,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,19 +2278,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,19 +2298,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2322,8 +2337,8 @@
   </sheetPr>
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2335,99 +2350,99 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="19" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,7 +2459,7 @@
         <v>50000000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>2000000</v>
@@ -2453,34 +2468,34 @@
         <v>3000000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="R2" s="1" t="n">
         <v>1232141241</v>
@@ -2489,7 +2504,7 @@
         <v>15000000</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="U2" s="1" t="n">
         <v>2024</v>
@@ -2501,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="Y2" s="1" t="n">
         <v>2024</v>
@@ -2513,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="AC2" s="1" t="n">
         <v>2024</v>
@@ -2539,7 +2554,7 @@
         <v>50000000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>2000000</v>
@@ -2548,34 +2563,34 @@
         <v>3000000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="R3" s="1" t="n">
         <v>1232141241</v>
@@ -2584,7 +2599,7 @@
         <v>15000000</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="U3" s="1" t="n">
         <v>2024</v>
@@ -2596,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="Y3" s="1" t="n">
         <v>2024</v>
@@ -2608,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AC3" s="1" t="n">
         <v>2024</v>
@@ -2634,7 +2649,7 @@
         <v>50000000</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2000000</v>
@@ -2643,34 +2658,34 @@
         <v>3000000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>1232141241</v>
@@ -2679,7 +2694,7 @@
         <v>15000000</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="U4" s="1" t="n">
         <v>2024</v>
@@ -2691,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>2024</v>
@@ -2703,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="AC4" s="1" t="n">
         <v>2024</v>
@@ -2729,7 +2744,7 @@
         <v>50000000</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2000000</v>
@@ -2738,34 +2753,34 @@
         <v>3000000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="R5" s="1" t="n">
         <v>1232141241</v>
@@ -2774,7 +2789,7 @@
         <v>15000000</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>2024</v>
@@ -2786,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="Y5" s="1" t="n">
         <v>2024</v>
@@ -2798,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AC5" s="1" t="n">
         <v>2024</v>
@@ -2828,8 +2843,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2843,30 +2858,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,7 +2889,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1242142151</v>
@@ -2886,13 +2901,13 @@
         <v>72686</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,7 +2915,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1242142151</v>
@@ -2912,13 +2927,13 @@
         <v>72686</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1242142151</v>
@@ -2938,13 +2953,13 @@
         <v>72686</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,7 +2967,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1242142151</v>
@@ -2964,13 +2979,13 @@
         <v>72686</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3008,78 +3023,78 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="21" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,25 +3102,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>0</v>
@@ -3114,16 +3129,16 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,25 +3146,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>0</v>
@@ -3158,16 +3173,16 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,25 +3190,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>0</v>
@@ -3202,16 +3217,16 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,25 +3234,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>0</v>
@@ -3246,16 +3261,16 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
company customer address page
</commit_message>
<xml_diff>
--- a/Data Files/LOS_CompanyCustomer_TestData.xlsx
+++ b/Data Files/LOS_CompanyCustomer_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="204">
   <si>
     <t xml:space="preserve">ScenarioId</t>
   </si>
@@ -258,6 +258,9 @@
     <t xml:space="preserve">JL DMSAIFSA1</t>
   </si>
   <si>
+    <t xml:space="preserve">15820</t>
+  </si>
+  <si>
     <t xml:space="preserve">BABAKAN</t>
   </si>
   <si>
@@ -279,6 +282,9 @@
     <t xml:space="preserve">Milik Sendiri</t>
   </si>
   <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
     <t xml:space="preserve">desc1</t>
   </si>
   <si>
@@ -292,6 +298,9 @@
   </si>
   <si>
     <t xml:space="preserve">JL DMSAIFSA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">BABAT</t>
@@ -1067,7 +1076,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1198,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1410,15 +1419,25 @@
   </sheetPr>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="4" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="28.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="11" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.65"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,56 +1515,56 @@
       <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>15820</v>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,61 +1572,61 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>15820</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,56 +1639,56 @@
       <c r="C4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>15820</v>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1" t="n">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1677,61 +1696,61 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>15820</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,56 +1763,56 @@
       <c r="C6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>15820</v>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,61 +1820,61 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>15820</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,56 +1887,56 @@
       <c r="C8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>15820</v>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1" t="n">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,61 +1944,61 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>15820</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2018,19 +2037,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,10 +2057,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>60</v>
@@ -2060,10 +2079,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>40</v>
@@ -2082,10 +2101,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>100</v>
@@ -2104,10 +2123,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>60</v>
@@ -2126,10 +2145,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>40</v>
@@ -2148,10 +2167,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>100</v>
@@ -2200,19 +2219,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>64</v>
@@ -2227,10 +2246,10 @@
         <v>67</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,19 +2257,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,19 +2277,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,19 +2297,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,19 +2317,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2355,94 +2374,94 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,7 +2478,7 @@
         <v>50000000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>2000000</v>
@@ -2468,34 +2487,34 @@
         <v>3000000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R2" s="1" t="n">
         <v>1232141241</v>
@@ -2504,7 +2523,7 @@
         <v>15000000</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="U2" s="1" t="n">
         <v>2024</v>
@@ -2516,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="Y2" s="1" t="n">
         <v>2024</v>
@@ -2528,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AC2" s="1" t="n">
         <v>2024</v>
@@ -2554,7 +2573,7 @@
         <v>50000000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>2000000</v>
@@ -2563,34 +2582,34 @@
         <v>3000000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R3" s="1" t="n">
         <v>1232141241</v>
@@ -2599,7 +2618,7 @@
         <v>15000000</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="U3" s="1" t="n">
         <v>2024</v>
@@ -2611,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Y3" s="1" t="n">
         <v>2024</v>
@@ -2623,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AC3" s="1" t="n">
         <v>2024</v>
@@ -2649,7 +2668,7 @@
         <v>50000000</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2000000</v>
@@ -2658,34 +2677,34 @@
         <v>3000000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>1232141241</v>
@@ -2694,7 +2713,7 @@
         <v>15000000</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="U4" s="1" t="n">
         <v>2024</v>
@@ -2706,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>2024</v>
@@ -2718,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AC4" s="1" t="n">
         <v>2024</v>
@@ -2744,7 +2763,7 @@
         <v>50000000</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2000000</v>
@@ -2753,34 +2772,34 @@
         <v>3000000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>12314141</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R5" s="1" t="n">
         <v>1232141241</v>
@@ -2789,7 +2808,7 @@
         <v>15000000</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>2024</v>
@@ -2801,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Y5" s="1" t="n">
         <v>2024</v>
@@ -2813,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AC5" s="1" t="n">
         <v>2024</v>
@@ -2863,25 +2882,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2889,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1242142151</v>
@@ -2901,13 +2920,13 @@
         <v>72686</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +2934,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1242142151</v>
@@ -2927,13 +2946,13 @@
         <v>72686</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,7 +2960,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1242142151</v>
@@ -2953,13 +2972,13 @@
         <v>72686</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,7 +2986,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1242142151</v>
@@ -2979,13 +2998,13 @@
         <v>72686</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3028,73 +3047,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3102,25 +3121,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>0</v>
@@ -3129,16 +3148,16 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,25 +3165,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>0</v>
@@ -3173,16 +3192,16 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,25 +3209,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>0</v>
@@ -3217,16 +3236,16 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3234,25 +3253,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>0</v>
@@ -3261,16 +3280,16 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>